<commit_message>
Customization of data dictionary
</commit_message>
<xml_diff>
--- a/demos/demo-data-dictionary/data-dictionary.xlsx
+++ b/demos/demo-data-dictionary/data-dictionary.xlsx
@@ -8,11 +8,14 @@
   <sheets>
     <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Sheet0!$A$1:$H$7</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Filename</t>
   </si>
@@ -47,9 +50,6 @@
     <t>some_column</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>varchar(200)</t>
   </si>
   <si>
@@ -59,13 +59,14 @@
     <t>some_other_column</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>some description
+with multiple lines</t>
   </si>
   <si>
     <t>xyz</t>
@@ -125,12 +126,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FF585858"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FF585858"/>
       </patternFill>
     </fill>
     <fill>
@@ -178,10 +179,18 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -196,12 +205,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="50"/>
   <cols>
-    <col min="1" max="1" width="15.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.01953125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="10.50390625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.2734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.0" customWidth="true"/>
+    <col min="2" max="2" width="20.0" customWidth="true"/>
+    <col min="3" max="3" width="12.0" customWidth="true"/>
+    <col min="4" max="4" width="12.0" customWidth="true"/>
+    <col min="5" max="5" width="14.0" customWidth="true"/>
+    <col min="6" max="6" width="12.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -251,14 +260,14 @@
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -269,26 +278,28 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -296,31 +307,32 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
+      <c r="C6" s="3" t="n">
+        <v>1.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H7"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Customizing data dictionary with alignment
</commit_message>
<xml_diff>
--- a/demos/demo-data-dictionary/data-dictionary.xlsx
+++ b/demos/demo-data-dictionary/data-dictionary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Filename</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>some_other_column</t>
@@ -86,13 +89,57 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="9"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="9.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -177,19 +224,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="left" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="left" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="left" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="left" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="right" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="right" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="right" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="right" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -219,7 +290,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -234,7 +305,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -259,7 +330,7 @@
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="8" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -268,37 +339,45 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="n">
         <v>2.0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -306,29 +385,35 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="7" t="n">
         <v>1.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H7"/>

</xml_diff>

<commit_message>
Setting sheet name in Excel
</commit_message>
<xml_diff>
--- a/demos/demo-data-dictionary/data-dictionary.xlsx
+++ b/demos/demo-data-dictionary/data-dictionary.xlsx
@@ -6,10 +6,10 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
+    <sheet name="Data Dictionary" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Sheet0!$A$1:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Data Dictionary'!$A$1:$H$7</definedName>
   </definedNames>
 </workbook>
 </file>

</xml_diff>